<commit_message>
drag drop input ok
</commit_message>
<xml_diff>
--- a/Offer.xlsx
+++ b/Offer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Programming\React-Projects\configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D19D7D-5720-4C65-8B17-39002A8256C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D48C9F8-2E98-4BA3-B648-2CFB21E5889F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EE1C98E-CE4C-4B52-8B05-8F072AB6EE4E}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{1EE1C98E-CE4C-4B52-8B05-8F072AB6EE4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,11 +610,11 @@
         <v>27</v>
       </c>
       <c r="B5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>240</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>30</v>
@@ -625,11 +625,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -715,11 +715,11 @@
         <v>15</v>
       </c>
       <c r="B12" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D12" s="5"/>
     </row>

</xml_diff>